<commit_message>
added 5 -other- categories. I thought this was added before but i guess i forgot --very strange
</commit_message>
<xml_diff>
--- a/fileShareApp/static/files_utility/categories.xlsx
+++ b/fileShareApp/static/files_utility/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210610kmDashboard2.0/fileShareApp/static/files_utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECACC07B-0190-4B4B-831C-A0D7C3B4A946}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC1CE5DC-87FF-4222-A856-E96B404E75AB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
+    <workbookView xWindow="25080" yWindow="-510" windowWidth="29040" windowHeight="15840" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t>Adavance Safety Issues</t>
   </si>
@@ -724,6 +724,24 @@
   </si>
   <si>
     <t>REMOTE_ENGINE_STARTS_BY_ITSELF</t>
+  </si>
+  <si>
+    <t>BRAKING_OTHER</t>
+  </si>
+  <si>
+    <t>HEADLIGHT_OTHER</t>
+  </si>
+  <si>
+    <t>EXTERIOR_LIGHTING_OTHER</t>
+  </si>
+  <si>
+    <t>SEATBELT_OTHER</t>
+  </si>
+  <si>
+    <t>SEAT_OTHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRES_OTHER </t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1164,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,6 +1485,9 @@
       <c r="N5" t="s">
         <v>164</v>
       </c>
+      <c r="O5" t="s">
+        <v>234</v>
+      </c>
       <c r="P5" t="s">
         <v>173</v>
       </c>
@@ -1736,11 +1757,17 @@
       <c r="H12" t="s">
         <v>78</v>
       </c>
+      <c r="I12" t="s">
+        <v>231</v>
+      </c>
       <c r="J12" t="s">
         <v>107</v>
       </c>
       <c r="M12" t="s">
         <v>137</v>
+      </c>
+      <c r="P12" t="s">
+        <v>233</v>
       </c>
       <c r="U12" t="s">
         <v>217</v>
@@ -1753,8 +1780,14 @@
       <c r="C13" t="s">
         <v>37</v>
       </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
       <c r="H13" t="s">
         <v>79</v>
+      </c>
+      <c r="I13" t="s">
+        <v>232</v>
       </c>
       <c r="J13" t="s">
         <v>108</v>
@@ -1837,6 +1870,9 @@
       </c>
     </row>
     <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>235</v>
+      </c>
       <c r="M19" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
saving progress: re organizing hosting machines
</commit_message>
<xml_diff>
--- a/fileShareApp/static/files_utility/categories.xlsx
+++ b/fileShareApp/static/files_utility/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210610kmDashboard2.0/fileShareApp/static/files_utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC1CE5DC-87FF-4222-A856-E96B404E75AB}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7250467F-6CAD-4FFB-AC74-F56931CE9F8C}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-510" windowWidth="29040" windowHeight="15840" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
   <si>
     <t>Adavance Safety Issues</t>
   </si>
@@ -742,6 +742,12 @@
   </si>
   <si>
     <t xml:space="preserve">FIRES_OTHER </t>
+  </si>
+  <si>
+    <t>DOOR_ISSUES_OTHER</t>
+  </si>
+  <si>
+    <t>BODY_GENERAL_ISSUES_OTHER</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1170,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,6 +1661,9 @@
       <c r="D9" t="s">
         <v>49</v>
       </c>
+      <c r="F9" t="s">
+        <v>236</v>
+      </c>
       <c r="H9" t="s">
         <v>75</v>
       </c>
@@ -1847,7 +1856,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>237</v>
+      </c>
       <c r="H17" t="s">
         <v>83</v>
       </c>
@@ -1858,7 +1870,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
         <v>84</v>
       </c>
@@ -1869,7 +1881,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>235</v>
       </c>
@@ -1877,67 +1889,67 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M32" t="s">
         <v>157</v>
       </c>

</xml_diff>

<commit_message>
report update: converted linked_records column from json string to using respective NHTSA_ACTION_Number or recrod_id
</commit_message>
<xml_diff>
--- a/fileShareApp/static/files_utility/categories.xlsx
+++ b/fileShareApp/static/files_utility/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210610kmDashboard2.0/fileShareApp/static/files_utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7250467F-6CAD-4FFB-AC74-F56931CE9F8C}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86B2F2E6-F199-45EB-96A0-474516437C54}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
+    <workbookView xWindow="29370" yWindow="3255" windowWidth="21630" windowHeight="9165" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
   <si>
     <t>Adavance Safety Issues</t>
   </si>
@@ -748,6 +748,18 @@
   </si>
   <si>
     <t>BODY_GENERAL_ISSUES_OTHER</t>
+  </si>
+  <si>
+    <t>AB_ISSUES_OTHER</t>
+  </si>
+  <si>
+    <t>WINDOWS_OTHER</t>
+  </si>
+  <si>
+    <t>WINDSHIELD_OTHER</t>
+  </si>
+  <si>
+    <t>ENGINE_TROUBLES_OTHER</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66008A2E-88F0-47BB-BD6C-411B302D29B6}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,11 +1735,17 @@
       <c r="U10" t="s">
         <v>215</v>
       </c>
+      <c r="V10" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
@@ -1751,6 +1769,9 @@
       </c>
       <c r="U11" t="s">
         <v>216</v>
+      </c>
+      <c r="V11" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1882,6 +1903,9 @@
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>241</v>
+      </c>
       <c r="J19" t="s">
         <v>235</v>
       </c>

</xml_diff>

<commit_message>
functionality update: if files_database doesnt exists, make it
</commit_message>
<xml_diff>
--- a/fileShareApp/static/files_utility/categories.xlsx
+++ b/fileShareApp/static/files_utility/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210610kmDashboard2.0/fileShareApp/static/files_utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86B2F2E6-F199-45EB-96A0-474516437C54}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EEDEA5-8636-41DD-BFE8-E0E7B8D36E27}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="3255" windowWidth="21630" windowHeight="9165" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
+    <workbookView xWindow="28740" yWindow="1425" windowWidth="21630" windowHeight="10920" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>Adavance Safety Issues</t>
   </si>
@@ -760,6 +760,12 @@
   </si>
   <si>
     <t>ENGINE_TROUBLES_OTHER</t>
+  </si>
+  <si>
+    <t>HOOD_ISSUES_OTHER</t>
+  </si>
+  <si>
+    <t>ROOF_RAIL_ISSUES_OTHER</t>
   </si>
 </sst>
 </file>
@@ -1181,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66008A2E-88F0-47BB-BD6C-411B302D29B6}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,11 +1556,17 @@
       <c r="J6" t="s">
         <v>101</v>
       </c>
+      <c r="K6" t="s">
+        <v>242</v>
+      </c>
       <c r="L6" t="s">
         <v>124</v>
       </c>
       <c r="M6" t="s">
         <v>131</v>
+      </c>
+      <c r="N6" t="s">
+        <v>243</v>
       </c>
       <c r="P6" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
functionality update: reports page remove id and record_id as column options. id and record_id always in table - otherwise there are problems building the excel file.
</commit_message>
<xml_diff>
--- a/fileShareApp/static/files_utility/categories.xlsx
+++ b/fileShareApp/static/files_utility/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210610kmDashboard2.0/fileShareApp/static/files_utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EEDEA5-8636-41DD-BFE8-E0E7B8D36E27}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{C7BF1B44-C626-4D9B-A996-5025C9F783A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC4744B-65CF-4205-AB31-640B53F81332}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="1425" windowWidth="21630" windowHeight="10920" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
+    <workbookView xWindow="27210" yWindow="2730" windowWidth="21630" windowHeight="10920" xr2:uid="{082F89AC-00E3-4EFA-898D-92CAE37F526D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>Instrument Panel Issues</t>
   </si>
   <si>
-    <t xml:space="preserve">VISIBILITY_ISSUES </t>
-  </si>
-  <si>
     <t>SPEEDOMETER_ISSUES</t>
   </si>
   <si>
@@ -504,9 +501,6 @@
     <t>AB_OCS_PILLOW_USAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">DRIVELINE_NOISE </t>
-  </si>
-  <si>
     <t>WARRANTY_COST</t>
   </si>
   <si>
@@ -558,9 +552,6 @@
     <t>SB_RETRACTOR_DOES_NOT_RETRACT</t>
   </si>
   <si>
-    <t xml:space="preserve">SB_RETRACTOR_DOES_NOT_LOCK </t>
-  </si>
-  <si>
     <t>SB_RETRACTOR_DOES_NOT_LOCK_WHILE_DRIVING</t>
   </si>
   <si>
@@ -741,9 +732,6 @@
     <t>SEAT_OTHER</t>
   </si>
   <si>
-    <t xml:space="preserve">FIRES_OTHER </t>
-  </si>
-  <si>
     <t>DOOR_ISSUES_OTHER</t>
   </si>
   <si>
@@ -766,6 +754,18 @@
   </si>
   <si>
     <t>ROOF_RAIL_ISSUES_OTHER</t>
+  </si>
+  <si>
+    <t>FIRES_OTHER</t>
+  </si>
+  <si>
+    <t>VISIBILITY_ISSUES</t>
+  </si>
+  <si>
+    <t>DRIVELINE_NOISE</t>
+  </si>
+  <si>
+    <t>SB_RETRACTOR_DOES_NOT_LOCK</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1188,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,34 +1244,34 @@
         <v>119</v>
       </c>
       <c r="M1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="S1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="T1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="U1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="V1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -1309,37 +1309,37 @@
         <v>114</v>
       </c>
       <c r="L2" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="R2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="S2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="T2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="U2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="V2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1374,37 +1374,37 @@
         <v>115</v>
       </c>
       <c r="L3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="S3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="T3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="U3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="V3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1439,37 +1439,37 @@
         <v>116</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="R4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="S4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="T4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="U4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="V4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1501,34 +1501,34 @@
         <v>117</v>
       </c>
       <c r="L5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="P5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="T5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="U5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="V5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1557,34 +1557,34 @@
         <v>101</v>
       </c>
       <c r="K6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="L6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N6" t="s">
+        <v>239</v>
+      </c>
+      <c r="P6" t="s">
         <v>243</v>
       </c>
-      <c r="P6" t="s">
-        <v>174</v>
-      </c>
       <c r="Q6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="S6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="T6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="U6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="V6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1613,22 +1613,22 @@
         <v>102</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="U7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1657,19 +1657,19 @@
         <v>103</v>
       </c>
       <c r="M8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="S8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="V8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H9" t="s">
         <v>75</v>
@@ -1698,19 +1698,19 @@
         <v>104</v>
       </c>
       <c r="M9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="S9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="U9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="V9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1736,19 +1736,19 @@
         <v>105</v>
       </c>
       <c r="M10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="U10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="V10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
@@ -1774,16 +1774,16 @@
         <v>106</v>
       </c>
       <c r="M11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="V11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1800,19 +1800,19 @@
         <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J12" t="s">
         <v>107</v>
       </c>
       <c r="M12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P12" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="U12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1823,22 +1823,22 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H13" t="s">
         <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J13" t="s">
         <v>108</v>
       </c>
       <c r="M13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>109</v>
       </c>
       <c r="M14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
         <v>110</v>
       </c>
       <c r="M15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1886,12 +1886,12 @@
         <v>111</v>
       </c>
       <c r="M16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H17" t="s">
         <v>83</v>
@@ -1900,7 +1900,7 @@
         <v>112</v>
       </c>
       <c r="M17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
@@ -1911,103 +1911,103 @@
         <v>113</v>
       </c>
       <c r="M18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J19" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
-        <v>156</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>